<commit_message>
added additional demographic team columns and corrected naive linear forecasts
</commit_message>
<xml_diff>
--- a/Data Cleaning/demo_check.xlsx
+++ b/Data Cleaning/demo_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/Data Cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E56B99EF-F381-4FD2-AAAE-1273F3777E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{195AF519-7C99-4AFE-85DE-F0067ECAB900}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{E56B99EF-F381-4FD2-AAAE-1273F3777E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1773FCD0-9954-468F-8BD7-CF10577F8B7C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="1029">
   <si>
     <t>ResponseId</t>
   </si>
@@ -2731,60 +2731,12 @@
     <t>Judgemental Forecasting, Project Management</t>
   </si>
   <si>
-    <t>Might be Bilge Gencoglu at University of Groningen</t>
-  </si>
-  <si>
-    <t>Nathan Dhaliwal of UBC?</t>
-  </si>
-  <si>
-    <t>J.M. Tybur of VUA</t>
-  </si>
-  <si>
     <t>Ishan Singhal</t>
   </si>
   <si>
-    <t>scott-janzwood at balsilie school of international affairs</t>
-  </si>
-  <si>
-    <t>Pascal Boyer, washington university in st louis</t>
-  </si>
-  <si>
-    <t>Dr. Dan Lannin at Illinois State University</t>
-  </si>
-  <si>
-    <t>Dr. Hong Miao, Colorado State University</t>
-  </si>
-  <si>
-    <t>Anoosha Izadi, umass dartmouth</t>
-  </si>
-  <si>
     <t>Mariola Paruzel-Czachura</t>
   </si>
   <si>
-    <t>Jared B Kenworthy, University of Texas</t>
-  </si>
-  <si>
-    <t>Yukiko Uchida, Kyoto University</t>
-  </si>
-  <si>
-    <t>Nigel Mantou Lou, was at McGill, now at Uvic</t>
-  </si>
-  <si>
-    <t>Bethany A. Teachman, University of Virginia</t>
-  </si>
-  <si>
-    <t>Maximilian Maier at UCL</t>
-  </si>
-  <si>
-    <t>Peter Slattery, Monash</t>
-  </si>
-  <si>
-    <t>Joanna Swartz, at UC Davis</t>
-  </si>
-  <si>
-    <t>Anton Gollwitzer, Yale</t>
-  </si>
-  <si>
     <t>Moral psychology</t>
   </si>
   <si>
@@ -2797,18 +2749,9 @@
     <t>Landy et al. (2020), Psychological Bulletin.</t>
   </si>
   <si>
-    <t>Dr Chung-Ching Tai, University of South Hampton</t>
-  </si>
-  <si>
     <t>Disciplinary_Orientation</t>
   </si>
   <si>
-    <t xml:space="preserve"> i. behavioral sciences;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ii. social sciences;</t>
-  </si>
-  <si>
     <t>The team has expertise in the area of daily events that encompass prosocial acts, the effects of various daily occurrences on subjective well-being, as well as a range of research in the area of executive functions and self-regulation. Collectively, the team has published more than 30 peer-reviewed jourl articles in these areas.</t>
   </si>
   <si>
@@ -2839,15 +2782,6 @@
     <t>Psych Methods, Computer Science</t>
   </si>
   <si>
-    <t>v. other</t>
-  </si>
-  <si>
-    <t>iv. Interdisciplinary</t>
-  </si>
-  <si>
-    <t>Amanda</t>
-  </si>
-  <si>
     <t>Nadyanna M. Majeed</t>
   </si>
   <si>
@@ -2971,9 +2905,6 @@
     <t>Austria</t>
   </si>
   <si>
-    <t>Eric Shuman (team leader)</t>
-  </si>
-  <si>
     <t>Social Psychology/Intergroup Relations</t>
   </si>
   <si>
@@ -3079,9 +3010,6 @@
     <t>David Jimenez-Gomez</t>
   </si>
   <si>
-    <t>David Jimenez-Gomez, University of Alicante - manually filled in all information aside from email</t>
-  </si>
-  <si>
     <t>Business, Economics</t>
   </si>
   <si>
@@ -3115,9 +3043,6 @@
     <t>Quantitative &amp; Empirical Finance</t>
   </si>
   <si>
-    <t xml:space="preserve"> iii. Data &amp; computer sciences; </t>
-  </si>
-  <si>
     <t>Hong Miao</t>
   </si>
   <si>
@@ -3130,9 +3055,6 @@
     <t>Linguistics, language &amp; culture</t>
   </si>
   <si>
-    <t>Unable to identify</t>
-  </si>
-  <si>
     <t>non-binary</t>
   </si>
   <si>
@@ -3167,6 +3089,39 @@
   </si>
   <si>
     <t>Manually Added (1 = added all info aside from email/name, 2 = added expertise)</t>
+  </si>
+  <si>
+    <t>Monica Thieu</t>
+  </si>
+  <si>
+    <t>monica.thieu@columbia.edu</t>
+  </si>
+  <si>
+    <t>Social neuroscience</t>
+  </si>
+  <si>
+    <t>Matthew Hornsey</t>
+  </si>
+  <si>
+    <t>m.hornsey@uq.edu.au</t>
+  </si>
+  <si>
+    <t>intergroup relations</t>
+  </si>
+  <si>
+    <t>social influence</t>
+  </si>
+  <si>
+    <t>petertslattery@gmail.com</t>
+  </si>
+  <si>
+    <t>Behaviour Change</t>
+  </si>
+  <si>
+    <t>Eric Shuman</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -4104,11 +4059,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF191"/>
+  <dimension ref="A1:AB191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W23" sqref="W23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4073,7 @@
     <col min="21" max="21" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4180,7 +4135,7 @@
         <v>730</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>927</v>
+        <v>908</v>
       </c>
       <c r="V1" t="s">
         <v>17</v>
@@ -4189,22 +4144,22 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>993</v>
+        <v>970</v>
       </c>
       <c r="Y1" t="s">
-        <v>921</v>
+        <v>904</v>
       </c>
       <c r="Z1" t="s">
         <v>725</v>
       </c>
       <c r="AA1" t="s">
-        <v>1043</v>
+        <v>1017</v>
       </c>
       <c r="AB1" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4262,11 +4217,8 @@
       <c r="Z2">
         <v>0</v>
       </c>
-      <c r="AD2" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -4321,11 +4273,8 @@
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AD3" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4380,11 +4329,8 @@
       <c r="Z4">
         <v>0</v>
       </c>
-      <c r="AD4" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -4439,11 +4385,8 @@
       <c r="Z5">
         <v>0</v>
       </c>
-      <c r="AD5" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -4460,16 +4403,16 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>1022</v>
+        <v>998</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>976</v>
+        <v>954</v>
       </c>
       <c r="H6" s="4">
         <v>26</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>977</v>
+        <v>955</v>
       </c>
       <c r="J6" s="4">
         <v>1</v>
@@ -4493,7 +4436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -4510,7 +4453,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>937</v>
+        <v>915</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>37</v>
@@ -4537,7 +4480,7 @@
         <v>153</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>924</v>
+        <v>905</v>
       </c>
       <c r="V7" s="4">
         <v>2</v>
@@ -4548,14 +4491,8 @@
       <c r="Z7" s="4">
         <v>0</v>
       </c>
-      <c r="AB7" s="4" t="s">
-        <v>937</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
@@ -4572,10 +4509,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>961</v>
+        <v>939</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>962</v>
+        <v>940</v>
       </c>
       <c r="H8" s="4">
         <v>21</v>
@@ -4608,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -4625,10 +4562,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>963</v>
+        <v>941</v>
       </c>
       <c r="G9" t="s">
-        <v>964</v>
+        <v>942</v>
       </c>
       <c r="H9">
         <v>29</v>
@@ -4649,10 +4586,10 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>965</v>
+        <v>943</v>
       </c>
       <c r="T9" t="s">
-        <v>966</v>
+        <v>944</v>
       </c>
       <c r="V9">
         <v>2</v>
@@ -4664,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
@@ -4681,10 +4618,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>967</v>
+        <v>945</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>968</v>
+        <v>946</v>
       </c>
       <c r="H10" s="4">
         <v>24</v>
@@ -4705,7 +4642,7 @@
         <v>1</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>994</v>
+        <v>971</v>
       </c>
       <c r="Y10" s="4">
         <v>4</v>
@@ -4714,7 +4651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -4731,10 +4668,10 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>969</v>
+        <v>947</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>970</v>
+        <v>948</v>
       </c>
       <c r="H11">
         <v>24</v>
@@ -4758,7 +4695,7 @@
         <v>153</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>995</v>
+        <v>972</v>
       </c>
       <c r="V11">
         <v>2</v>
@@ -4770,7 +4707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -4787,7 +4724,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1000</v>
+        <v>977</v>
       </c>
       <c r="H12" s="4">
         <v>25</v>
@@ -4814,7 +4751,7 @@
         <v>153</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>1001</v>
+        <v>978</v>
       </c>
       <c r="V12" s="4">
         <v>2</v>
@@ -4828,11 +4765,8 @@
       <c r="AA12" s="4">
         <v>1</v>
       </c>
-      <c r="AB12" s="4" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -4849,10 +4783,10 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>991</v>
+        <v>968</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>992</v>
+        <v>969</v>
       </c>
       <c r="I13" t="s">
         <v>148</v>
@@ -4870,7 +4804,7 @@
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>990</v>
+        <v>967</v>
       </c>
       <c r="V13">
         <v>2</v>
@@ -4881,11 +4815,8 @@
       <c r="Z13">
         <v>0</v>
       </c>
-      <c r="AB13" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -4944,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -4961,11 +4892,14 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>1023</v>
+        <v>999</v>
       </c>
       <c r="G15" t="s">
         <v>52</v>
       </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
       <c r="J15">
         <v>4</v>
       </c>
@@ -4988,7 +4922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -5005,10 +4939,10 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>1019</v>
+        <v>995</v>
       </c>
       <c r="G16" t="s">
-        <v>1020</v>
+        <v>996</v>
       </c>
       <c r="H16">
         <v>28</v>
@@ -5029,7 +4963,7 @@
         <v>3</v>
       </c>
       <c r="R16" t="s">
-        <v>1021</v>
+        <v>997</v>
       </c>
       <c r="U16" s="3" t="s">
         <v>184</v>
@@ -5044,7 +4978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -5103,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -5120,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>974</v>
+        <v>952</v>
       </c>
       <c r="G18" t="s">
         <v>58</v>
@@ -5153,7 +5087,7 @@
         <v>1</v>
       </c>
       <c r="W18" t="s">
-        <v>975</v>
+        <v>953</v>
       </c>
       <c r="Y18">
         <v>2</v>
@@ -5161,11 +5095,8 @@
       <c r="Z18">
         <v>0</v>
       </c>
-      <c r="AB18" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
@@ -5182,17 +5113,23 @@
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="I19" s="4" t="s">
+        <v>1028</v>
+      </c>
       <c r="J19" s="4">
         <v>3</v>
       </c>
       <c r="L19" s="4">
         <v>3</v>
       </c>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
       <c r="P19" s="4">
         <v>1</v>
       </c>
@@ -5209,13 +5146,10 @@
         <v>1</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>901</v>
-      </c>
-      <c r="AC19" s="4" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>62</v>
       </c>
@@ -5256,7 +5190,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>926</v>
+        <v>907</v>
       </c>
       <c r="V20" s="4">
         <v>2</v>
@@ -5271,7 +5205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -5312,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>925</v>
+        <v>906</v>
       </c>
       <c r="V21" s="4">
         <v>2</v>
@@ -5327,7 +5261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -5389,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -5454,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -5498,7 +5432,7 @@
         <v>85</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>1005</v>
+        <v>982</v>
       </c>
       <c r="V24">
         <v>2</v>
@@ -5510,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -5569,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>86</v>
       </c>
@@ -5610,7 +5544,7 @@
         <v>1</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>928</v>
+        <v>909</v>
       </c>
       <c r="V26" s="4">
         <v>2</v>
@@ -5625,7 +5559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -5681,7 +5615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>95</v>
       </c>
@@ -5734,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>95</v>
       </c>
@@ -5796,7 +5730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>105</v>
       </c>
@@ -5837,7 +5771,7 @@
         <v>1</v>
       </c>
       <c r="U30" s="4" t="s">
-        <v>1015</v>
+        <v>991</v>
       </c>
       <c r="V30" s="4">
         <v>2</v>
@@ -5852,7 +5786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>105</v>
       </c>
@@ -5911,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>105</v>
       </c>
@@ -5972,11 +5906,8 @@
       <c r="Z32" s="9">
         <v>3</v>
       </c>
-      <c r="AB32" s="9" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -5993,10 +5924,10 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>986</v>
+        <v>963</v>
       </c>
       <c r="G33" t="s">
-        <v>987</v>
+        <v>964</v>
       </c>
       <c r="H33">
         <v>48</v>
@@ -6017,10 +5948,10 @@
         <v>1</v>
       </c>
       <c r="R33" t="s">
-        <v>988</v>
+        <v>965</v>
       </c>
       <c r="S33" t="s">
-        <v>989</v>
+        <v>966</v>
       </c>
       <c r="V33">
         <v>2</v>
@@ -6029,11 +5960,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
       <c r="B34" t="s">
         <v>106</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>107</v>
       </c>
       <c r="D34">
@@ -6044,7 +5978,7 @@
       </c>
       <c r="Y34" s="9"/>
     </row>
-    <row r="35" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>114</v>
       </c>
@@ -6061,11 +5995,14 @@
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>1017</v>
+        <v>993</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="I35" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="J35" s="4">
         <v>4</v>
       </c>
@@ -6079,7 +6016,7 @@
         <v>1</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>1016</v>
+        <v>992</v>
       </c>
       <c r="Y35" s="4">
         <v>2</v>
@@ -6090,11 +6027,8 @@
       <c r="AA35" s="4">
         <v>1</v>
       </c>
-      <c r="AB35" s="4" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -6150,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>120</v>
       </c>
@@ -6167,7 +6101,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>1024</v>
+        <v>1000</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>122</v>
@@ -6188,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="U37" s="4" t="s">
-        <v>1018</v>
+        <v>994</v>
       </c>
       <c r="Y37" s="4">
         <v>2</v>
@@ -6199,11 +6133,8 @@
       <c r="AA37" s="4">
         <v>1</v>
       </c>
-      <c r="AB37" s="4" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -6262,7 +6193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -6327,7 +6258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -6344,7 +6275,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>950</v>
+        <v>928</v>
       </c>
       <c r="G40" t="s">
         <v>134</v>
@@ -6371,7 +6302,7 @@
         <v>153</v>
       </c>
       <c r="S40" t="s">
-        <v>951</v>
+        <v>929</v>
       </c>
       <c r="V40">
         <v>2</v>
@@ -6382,11 +6313,8 @@
       <c r="Z40">
         <v>0</v>
       </c>
-      <c r="AB40" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>135</v>
       </c>
@@ -6439,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>138</v>
       </c>
@@ -6492,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>144</v>
       </c>
@@ -6551,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -6607,7 +6535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>155</v>
       </c>
@@ -6666,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>161</v>
       </c>
@@ -6719,7 +6647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>161</v>
       </c>
@@ -6775,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>169</v>
       </c>
@@ -6792,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>1027</v>
+        <v>1002</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>171</v>
@@ -6813,7 +6741,7 @@
         <v>1</v>
       </c>
       <c r="U48" s="4" t="s">
-        <v>1025</v>
+        <v>1001</v>
       </c>
       <c r="Y48" s="4">
         <v>3</v>
@@ -6823,9 +6751,6 @@
       </c>
       <c r="AA48" s="4">
         <v>1</v>
-      </c>
-      <c r="AB48" s="4" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
@@ -7517,7 +7442,7 @@
         <v>3</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>1032</v>
+        <v>1006</v>
       </c>
       <c r="P61" s="4">
         <v>1</v>
@@ -7526,10 +7451,10 @@
         <v>26</v>
       </c>
       <c r="S61" t="s">
-        <v>1033</v>
+        <v>1007</v>
       </c>
       <c r="U61" s="4" t="s">
-        <v>1029</v>
+        <v>1004</v>
       </c>
       <c r="V61" s="4">
         <v>2</v>
@@ -7585,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="U62" s="4" t="s">
-        <v>1028</v>
+        <v>1003</v>
       </c>
       <c r="V62" s="4">
         <v>2</v>
@@ -7809,7 +7734,7 @@
         <v>1</v>
       </c>
       <c r="U66" s="4" t="s">
-        <v>1030</v>
+        <v>1005</v>
       </c>
       <c r="V66" s="4">
         <v>2</v>
@@ -8337,7 +8262,7 @@
         <v>127</v>
       </c>
       <c r="U75" s="4" t="s">
-        <v>1039</v>
+        <v>1013</v>
       </c>
       <c r="V75" s="4">
         <v>2</v>
@@ -8644,7 +8569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>304</v>
       </c>
@@ -8661,7 +8586,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="G81" t="s">
         <v>306</v>
@@ -8685,19 +8610,19 @@
         <v>1</v>
       </c>
       <c r="R81" t="s">
-        <v>916</v>
+        <v>900</v>
       </c>
       <c r="S81" t="s">
-        <v>917</v>
+        <v>901</v>
       </c>
       <c r="T81" t="s">
-        <v>918</v>
+        <v>902</v>
       </c>
       <c r="V81">
         <v>1</v>
       </c>
       <c r="W81" t="s">
-        <v>919</v>
+        <v>903</v>
       </c>
       <c r="Y81">
         <v>1</v>
@@ -8706,7 +8631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>307</v>
       </c>
@@ -8765,7 +8690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>307</v>
       </c>
@@ -8821,7 +8746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>315</v>
       </c>
@@ -8880,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>318</v>
       </c>
@@ -8939,7 +8864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>321</v>
       </c>
@@ -8998,7 +8923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>324</v>
       </c>
@@ -9057,7 +8982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>333</v>
       </c>
@@ -9110,7 +9035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>336</v>
       </c>
@@ -9169,7 +9094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>343</v>
       </c>
@@ -9231,7 +9156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>343</v>
       </c>
@@ -9245,7 +9170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>346</v>
       </c>
@@ -9301,7 +9226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>353</v>
       </c>
@@ -9354,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>356</v>
       </c>
@@ -9371,7 +9296,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>1034</v>
+        <v>1008</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>358</v>
@@ -9392,7 +9317,7 @@
         <v>1</v>
       </c>
       <c r="U94" s="4" t="s">
-        <v>929</v>
+        <v>910</v>
       </c>
       <c r="Y94" s="4">
         <v>2</v>
@@ -9403,11 +9328,8 @@
       <c r="AA94" s="4">
         <v>1</v>
       </c>
-      <c r="AB94" s="4" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>359</v>
       </c>
@@ -9424,16 +9346,16 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>982</v>
+        <v>959</v>
       </c>
       <c r="G95" t="s">
-        <v>983</v>
+        <v>960</v>
       </c>
       <c r="H95">
         <v>45</v>
       </c>
       <c r="I95" t="s">
-        <v>984</v>
+        <v>961</v>
       </c>
       <c r="J95">
         <v>4</v>
@@ -9451,13 +9373,13 @@
         <v>262</v>
       </c>
       <c r="U95" s="3" t="s">
-        <v>930</v>
+        <v>911</v>
       </c>
       <c r="V95">
         <v>1</v>
       </c>
       <c r="W95" t="s">
-        <v>985</v>
+        <v>962</v>
       </c>
       <c r="Y95">
         <v>2</v>
@@ -9465,11 +9387,8 @@
       <c r="Z95">
         <v>0</v>
       </c>
-      <c r="AB95" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>362</v>
       </c>
@@ -9531,7 +9450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>362</v>
       </c>
@@ -9593,7 +9512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>373</v>
       </c>
@@ -9649,7 +9568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>373</v>
       </c>
@@ -9705,7 +9624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>373</v>
       </c>
@@ -9761,7 +9680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>386</v>
       </c>
@@ -9820,7 +9739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>386</v>
       </c>
@@ -9876,7 +9795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>386</v>
       </c>
@@ -9935,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>403</v>
       </c>
@@ -9997,7 +9916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>406</v>
       </c>
@@ -10053,7 +9972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>409</v>
       </c>
@@ -10073,7 +9992,7 @@
         <v>410</v>
       </c>
       <c r="G106" t="s">
-        <v>955</v>
+        <v>933</v>
       </c>
       <c r="H106">
         <v>30</v>
@@ -10094,7 +10013,7 @@
         <v>1</v>
       </c>
       <c r="R106" t="s">
-        <v>956</v>
+        <v>934</v>
       </c>
       <c r="S106" t="s">
         <v>26</v>
@@ -10103,7 +10022,7 @@
         <v>2</v>
       </c>
       <c r="W106" t="s">
-        <v>931</v>
+        <v>912</v>
       </c>
       <c r="Y106">
         <v>2</v>
@@ -10111,11 +10030,8 @@
       <c r="Z106">
         <v>0</v>
       </c>
-      <c r="AB106" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>412</v>
       </c>
@@ -10168,7 +10084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>416</v>
       </c>
@@ -10185,7 +10101,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>957</v>
+        <v>935</v>
       </c>
       <c r="G108" t="s">
         <v>418</v>
@@ -10209,13 +10125,13 @@
         <v>1</v>
       </c>
       <c r="R108" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="S108" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="U108" t="s">
-        <v>932</v>
+        <v>913</v>
       </c>
       <c r="V108">
         <v>2</v>
@@ -10226,11 +10142,8 @@
       <c r="Z108">
         <v>0</v>
       </c>
-      <c r="AB108" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="109" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>419</v>
       </c>
@@ -10268,7 +10181,7 @@
         <v>1</v>
       </c>
       <c r="U109" s="4" t="s">
-        <v>933</v>
+        <v>914</v>
       </c>
       <c r="Y109" s="4">
         <v>3</v>
@@ -10279,11 +10192,8 @@
       <c r="AA109" s="4">
         <v>1</v>
       </c>
-      <c r="AB109" s="4" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>421</v>
       </c>
@@ -10345,7 +10255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>424</v>
       </c>
@@ -10398,7 +10308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>427</v>
       </c>
@@ -10457,7 +10367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>430</v>
       </c>
@@ -10516,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>438</v>
       </c>
@@ -10581,7 +10491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>447</v>
       </c>
@@ -10637,7 +10547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>453</v>
       </c>
@@ -10693,7 +10603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>453</v>
       </c>
@@ -10752,7 +10662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>463</v>
       </c>
@@ -10769,10 +10679,10 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>952</v>
+        <v>930</v>
       </c>
       <c r="G118" t="s">
-        <v>953</v>
+        <v>931</v>
       </c>
       <c r="H118">
         <v>34</v>
@@ -10793,7 +10703,7 @@
         <v>1</v>
       </c>
       <c r="R118" t="s">
-        <v>954</v>
+        <v>932</v>
       </c>
       <c r="V118">
         <v>2</v>
@@ -10804,11 +10714,8 @@
       <c r="Z118">
         <v>0</v>
       </c>
-      <c r="AB118" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>465</v>
       </c>
@@ -10827,7 +10734,7 @@
       <c r="F119" t="s">
         <v>468</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G119" s="2" t="s">
         <v>469</v>
       </c>
       <c r="H119">
@@ -10864,7 +10771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>465</v>
       </c>
@@ -10881,19 +10788,28 @@
         <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>978</v>
+        <v>1027</v>
       </c>
       <c r="G120" t="s">
         <v>467</v>
       </c>
+      <c r="I120" t="s">
+        <v>91</v>
+      </c>
       <c r="J120">
         <v>2</v>
       </c>
       <c r="L120">
         <v>3</v>
       </c>
+      <c r="N120">
+        <v>1</v>
+      </c>
+      <c r="P120">
+        <v>1</v>
+      </c>
       <c r="R120" t="s">
-        <v>979</v>
+        <v>956</v>
       </c>
       <c r="V120">
         <v>2</v>
@@ -10905,7 +10821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>473</v>
       </c>
@@ -10967,7 +10883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>473</v>
       </c>
@@ -11023,7 +10939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>484</v>
       </c>
@@ -11085,7 +11001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>491</v>
       </c>
@@ -11102,10 +11018,13 @@
         <v>1</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>999</v>
-      </c>
-      <c r="G124" s="4" t="s">
-        <v>493</v>
+        <v>976</v>
+      </c>
+      <c r="G124" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H124" s="4">
+        <v>34</v>
       </c>
       <c r="I124" s="4" t="s">
         <v>55</v>
@@ -11122,8 +11041,17 @@
       <c r="P124" s="4">
         <v>1</v>
       </c>
+      <c r="R124" t="s">
+        <v>1026</v>
+      </c>
+      <c r="S124" t="s">
+        <v>589</v>
+      </c>
       <c r="U124" s="4" t="s">
-        <v>998</v>
+        <v>975</v>
+      </c>
+      <c r="V124" s="4">
+        <v>2</v>
       </c>
       <c r="Y124" s="4">
         <v>4</v>
@@ -11134,11 +11062,8 @@
       <c r="AA124" s="4">
         <v>1</v>
       </c>
-      <c r="AB124" s="4" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>494</v>
       </c>
@@ -11191,7 +11116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>498</v>
       </c>
@@ -11247,7 +11172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>504</v>
       </c>
@@ -11306,7 +11231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>504</v>
       </c>
@@ -11323,10 +11248,10 @@
         <v>2</v>
       </c>
       <c r="F128" t="s">
-        <v>940</v>
+        <v>918</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>939</v>
+        <v>917</v>
       </c>
       <c r="I128" t="s">
         <v>148</v>
@@ -11344,10 +11269,10 @@
         <v>1</v>
       </c>
       <c r="R128" t="s">
-        <v>941</v>
+        <v>919</v>
       </c>
       <c r="S128" t="s">
-        <v>942</v>
+        <v>920</v>
       </c>
       <c r="V128">
         <v>2</v>
@@ -11359,7 +11284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>504</v>
       </c>
@@ -11376,10 +11301,10 @@
         <v>2</v>
       </c>
       <c r="F129" t="s">
-        <v>948</v>
+        <v>926</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>949</v>
+        <v>927</v>
       </c>
       <c r="H129">
         <v>37</v>
@@ -11412,7 +11337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>504</v>
       </c>
@@ -11429,10 +11354,10 @@
         <v>2</v>
       </c>
       <c r="F130" t="s">
-        <v>940</v>
+        <v>918</v>
       </c>
       <c r="G130" t="s">
-        <v>996</v>
+        <v>973</v>
       </c>
       <c r="H130">
         <v>35</v>
@@ -11453,7 +11378,7 @@
         <v>1</v>
       </c>
       <c r="R130" t="s">
-        <v>997</v>
+        <v>974</v>
       </c>
       <c r="S130" t="s">
         <v>153</v>
@@ -11468,7 +11393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>508</v>
       </c>
@@ -11485,7 +11410,7 @@
         <v>1</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>1013</v>
+        <v>990</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>510</v>
@@ -11506,7 +11431,7 @@
         <v>1</v>
       </c>
       <c r="U131" s="4" t="s">
-        <v>1012</v>
+        <v>989</v>
       </c>
       <c r="Y131" s="4">
         <v>2</v>
@@ -11517,11 +11442,8 @@
       <c r="AA131" s="4">
         <v>1</v>
       </c>
-      <c r="AB131" s="4" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>511</v>
       </c>
@@ -11580,7 +11502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>514</v>
       </c>
@@ -11639,7 +11561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>520</v>
       </c>
@@ -11661,11 +11583,8 @@
       <c r="AA134" s="4">
         <v>1</v>
       </c>
-      <c r="AB134" s="4" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>523</v>
       </c>
@@ -11721,7 +11640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>530</v>
       </c>
@@ -11777,7 +11696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>533</v>
       </c>
@@ -11832,11 +11751,8 @@
       <c r="Z137">
         <v>0</v>
       </c>
-      <c r="AF137" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>533</v>
       </c>
@@ -11895,7 +11811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>544</v>
       </c>
@@ -11912,7 +11828,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>980</v>
+        <v>957</v>
       </c>
       <c r="G139" t="s">
         <v>546</v>
@@ -11933,7 +11849,7 @@
         <v>1</v>
       </c>
       <c r="R139" s="6" t="s">
-        <v>981</v>
+        <v>958</v>
       </c>
       <c r="V139">
         <v>2</v>
@@ -11944,11 +11860,8 @@
       <c r="Z139">
         <v>0</v>
       </c>
-      <c r="AB139" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>547</v>
       </c>
@@ -12001,7 +11914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>547</v>
       </c>
@@ -12054,7 +11967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>547</v>
       </c>
@@ -12107,7 +12020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>547</v>
       </c>
@@ -12120,8 +12033,47 @@
       <c r="D143">
         <v>4</v>
       </c>
-    </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="F143" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G143" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H143">
+        <v>27</v>
+      </c>
+      <c r="I143" t="s">
+        <v>84</v>
+      </c>
+      <c r="J143">
+        <v>2</v>
+      </c>
+      <c r="L143">
+        <v>3</v>
+      </c>
+      <c r="N143">
+        <v>2</v>
+      </c>
+      <c r="P143">
+        <v>1</v>
+      </c>
+      <c r="R143" t="s">
+        <v>1020</v>
+      </c>
+      <c r="S143" t="s">
+        <v>452</v>
+      </c>
+      <c r="V143">
+        <v>2</v>
+      </c>
+      <c r="Y143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>555</v>
       </c>
@@ -12174,7 +12126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>555</v>
       </c>
@@ -12233,7 +12185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>555</v>
       </c>
@@ -12289,7 +12241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>569</v>
       </c>
@@ -12302,6 +12254,9 @@
       <c r="D147">
         <v>4</v>
       </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
       <c r="F147" t="s">
         <v>785</v>
       </c>
@@ -12342,7 +12297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>569</v>
       </c>
@@ -12383,7 +12338,7 @@
         <v>1</v>
       </c>
       <c r="U148" s="4" t="s">
-        <v>1035</v>
+        <v>1009</v>
       </c>
       <c r="V148" s="4">
         <v>2</v>
@@ -12398,7 +12353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>569</v>
       </c>
@@ -12439,7 +12394,7 @@
         <v>1</v>
       </c>
       <c r="U149" s="4" t="s">
-        <v>1036</v>
+        <v>1010</v>
       </c>
       <c r="V149" s="4">
         <v>2</v>
@@ -12454,7 +12409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>569</v>
       </c>
@@ -12495,7 +12450,7 @@
         <v>1</v>
       </c>
       <c r="U150" s="4" t="s">
-        <v>1037</v>
+        <v>1011</v>
       </c>
       <c r="V150" s="4">
         <v>2</v>
@@ -12510,7 +12465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>578</v>
       </c>
@@ -12566,7 +12521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>581</v>
       </c>
@@ -12583,10 +12538,10 @@
         <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>971</v>
+        <v>949</v>
       </c>
       <c r="G152" t="s">
-        <v>972</v>
+        <v>950</v>
       </c>
       <c r="H152">
         <v>28</v>
@@ -12610,7 +12565,7 @@
         <v>26</v>
       </c>
       <c r="S152" t="s">
-        <v>973</v>
+        <v>951</v>
       </c>
       <c r="V152">
         <v>2</v>
@@ -12621,11 +12576,8 @@
       <c r="Z152">
         <v>2</v>
       </c>
-      <c r="AB152" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>581</v>
       </c>
@@ -12639,7 +12591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>584</v>
       </c>
@@ -12695,7 +12647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>590</v>
       </c>
@@ -12757,7 +12709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>593</v>
       </c>
@@ -12774,7 +12726,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>1010</v>
+        <v>987</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>595</v>
@@ -12804,7 +12756,7 @@
         <v>598</v>
       </c>
       <c r="U156" s="3" t="s">
-        <v>1011</v>
+        <v>988</v>
       </c>
       <c r="V156">
         <v>1</v>
@@ -12819,7 +12771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>600</v>
       </c>
@@ -12878,7 +12830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>600</v>
       </c>
@@ -12937,7 +12889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>600</v>
       </c>
@@ -12996,7 +12948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>616</v>
       </c>
@@ -13298,6 +13250,9 @@
       <c r="D165">
         <v>4</v>
       </c>
+      <c r="E165">
+        <v>2</v>
+      </c>
       <c r="F165" t="s">
         <v>636</v>
       </c>
@@ -13323,10 +13278,10 @@
         <v>1</v>
       </c>
       <c r="R165" t="s">
-        <v>946</v>
+        <v>924</v>
       </c>
       <c r="S165" t="s">
-        <v>947</v>
+        <v>925</v>
       </c>
       <c r="V165">
         <v>2</v>
@@ -13351,8 +13306,11 @@
       <c r="D166">
         <v>4</v>
       </c>
+      <c r="E166">
+        <v>2</v>
+      </c>
       <c r="F166" s="7" t="s">
-        <v>943</v>
+        <v>921</v>
       </c>
       <c r="H166">
         <v>36</v>
@@ -13401,11 +13359,14 @@
       <c r="D167">
         <v>4</v>
       </c>
+      <c r="E167">
+        <v>2</v>
+      </c>
       <c r="F167" s="7" t="s">
-        <v>944</v>
+        <v>922</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>960</v>
+        <v>938</v>
       </c>
       <c r="H167">
         <v>35</v>
@@ -13426,7 +13387,7 @@
         <v>1</v>
       </c>
       <c r="R167" s="5" t="s">
-        <v>945</v>
+        <v>923</v>
       </c>
       <c r="V167">
         <v>2</v>
@@ -13600,7 +13561,7 @@
         <v>652</v>
       </c>
       <c r="U170" s="4" t="s">
-        <v>1009</v>
+        <v>986</v>
       </c>
       <c r="V170">
         <v>2</v>
@@ -13712,7 +13673,7 @@
         <v>49</v>
       </c>
       <c r="U172" s="4" t="s">
-        <v>1008</v>
+        <v>985</v>
       </c>
       <c r="V172" s="4">
         <v>2</v>
@@ -13771,7 +13732,7 @@
         <v>153</v>
       </c>
       <c r="U173" s="4" t="s">
-        <v>1007</v>
+        <v>984</v>
       </c>
       <c r="V173" s="4">
         <v>2</v>
@@ -14020,6 +13981,48 @@
       <c r="D178">
         <v>3</v>
       </c>
+      <c r="E178">
+        <v>2</v>
+      </c>
+      <c r="F178" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G178" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H178">
+        <v>48</v>
+      </c>
+      <c r="I178" t="s">
+        <v>55</v>
+      </c>
+      <c r="J178">
+        <v>4</v>
+      </c>
+      <c r="L178">
+        <v>4</v>
+      </c>
+      <c r="N178">
+        <v>1</v>
+      </c>
+      <c r="P178">
+        <v>1</v>
+      </c>
+      <c r="R178" t="s">
+        <v>1023</v>
+      </c>
+      <c r="S178" t="s">
+        <v>1024</v>
+      </c>
+      <c r="V178">
+        <v>2</v>
+      </c>
+      <c r="Y178">
+        <v>2</v>
+      </c>
+      <c r="Z178">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
@@ -14062,7 +14065,7 @@
         <v>1</v>
       </c>
       <c r="U179" s="4" t="s">
-        <v>1006</v>
+        <v>983</v>
       </c>
       <c r="V179" s="4">
         <v>2</v>
@@ -14206,7 +14209,10 @@
         <v>694</v>
       </c>
       <c r="D182">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>1</v>
       </c>
       <c r="F182" t="s">
         <v>869</v>
@@ -14342,7 +14348,7 @@
         <v>1</v>
       </c>
       <c r="U184" s="4" t="s">
-        <v>1004</v>
+        <v>981</v>
       </c>
       <c r="V184" s="4">
         <v>2</v>
@@ -14398,7 +14404,7 @@
         <v>1</v>
       </c>
       <c r="U185" s="4" t="s">
-        <v>1003</v>
+        <v>980</v>
       </c>
       <c r="V185" s="4">
         <v>2</v>
@@ -14454,7 +14460,7 @@
         <v>1</v>
       </c>
       <c r="U186" s="4" t="s">
-        <v>1002</v>
+        <v>979</v>
       </c>
       <c r="V186" s="4">
         <v>2</v>
@@ -14653,6 +14659,9 @@
       <c r="D190">
         <v>2</v>
       </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
       <c r="F190" t="s">
         <v>880</v>
       </c>
@@ -14709,7 +14718,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Z191" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="F1:F5 F181 F37:F38 F113:F117 F69:F70 F57:F58 F133:F135 F89 F148:F150 F40 F154 F54:F55 F137:F146 F111 F163 F42:F51 F79 F28:F31 F26 F94 F87 F85 F92 F183:F189 F35 F191:F1048576 F82:F83 F165 F156:F159 F161 F107 F60:F67 F131 F168:F179 F119 F109 F12:F15 F19:F24 F121:F127 F96:F103 F17 F73:F76">
+  <conditionalFormatting sqref="F1:F5 F181 F37:F38 F113:F117 F69:F70 F57:F58 F133:F135 F89 F148:F150 F40 F154 F54:F55 F137:F142 F111 F163 F42:F51 F79 F28:F31 F26 F94 F87 F85 F92 F183:F189 F35 F191:F1048576 F82:F83 F165 F156:F159 F161 F107 F60:F67 F131 F168:F177 F119 F109 F12:F15 F19:F24 F121:F127 F96:F103 F17 F73:F76 F144:F146 F179">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
@@ -14757,9 +14766,11 @@
     <hyperlink ref="G66" r:id="rId30" xr:uid="{80BAB38D-B7E9-4EE0-8E42-933F70281434}"/>
     <hyperlink ref="G94" r:id="rId31" xr:uid="{EB6560B3-E43B-4A09-9668-1B8DE0477FEC}"/>
     <hyperlink ref="C153" r:id="rId32" xr:uid="{4B7B91F3-CD8C-4E1A-92A6-8767C485960A}"/>
+    <hyperlink ref="G119" r:id="rId33" xr:uid="{B076B5D4-B3F9-45F0-AF2C-5F7CC3F4CC46}"/>
+    <hyperlink ref="C34" r:id="rId34" xr:uid="{24C2BAFA-8A4D-4DBA-81A7-5C1182C8B2CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 
@@ -14767,7 +14778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768622D9-9A80-4D10-B4C0-0D488149BD79}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
@@ -14784,16 +14795,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1040</v>
+        <v>1014</v>
       </c>
       <c r="E1" t="s">
-        <v>1041</v>
+        <v>1015</v>
       </c>
       <c r="F1" t="s">
-        <v>1038</v>
+        <v>1012</v>
       </c>
       <c r="G1" t="s">
-        <v>1042</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed MASE_w2 comparisons to linear & rwf naive forecasts
</commit_message>
<xml_diff>
--- a/Data Cleaning/demo_check.xlsx
+++ b/Data Cleaning/demo_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/ottwardu_uwaterloo_ca/Documents/Documents/GitHub/Forecasting-Tournament/Data Cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{E56B99EF-F381-4FD2-AAAE-1273F3777E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1773FCD0-9954-468F-8BD7-CF10577F8B7C}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{E56B99EF-F381-4FD2-AAAE-1273F3777E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0456301-4DE3-48DE-BCD5-5F9D42B2E26C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4063,7 +4063,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="K182" sqref="K182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,7 +5290,7 @@
         <v>70</v>
       </c>
       <c r="J22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
         <v>72</v>
@@ -5352,7 +5352,7 @@
         <v>25</v>
       </c>
       <c r="J23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K23" t="s">
         <v>77</v>
@@ -5874,7 +5874,7 @@
         <v>70</v>
       </c>
       <c r="J32" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>72</v>
@@ -7495,7 +7495,7 @@
         <v>55</v>
       </c>
       <c r="J62" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>233</v>
@@ -9479,7 +9479,7 @@
         <v>55</v>
       </c>
       <c r="J97">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K97" t="s">
         <v>371</v>
@@ -9883,7 +9883,7 @@
         <v>70</v>
       </c>
       <c r="J104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K104" t="s">
         <v>747</v>
@@ -12977,7 +12977,7 @@
         <v>70</v>
       </c>
       <c r="J160">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K160" t="s">
         <v>371</v>
@@ -13935,7 +13935,7 @@
         <v>55</v>
       </c>
       <c r="J177">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K177" t="s">
         <v>679</v>

</xml_diff>